<commit_message>
This is my third commit
</commit_message>
<xml_diff>
--- a/TestData/Excel.xlsx
+++ b/TestData/Excel.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4629" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6022" uniqueCount="134">
   <si>
     <t>Year</t>
   </si>
@@ -419,6 +419,18 @@
   </si>
   <si>
     <t>₹ 38,993</t>
+  </si>
+  <si>
+    <t>₹ 7,542</t>
+  </si>
+  <si>
+    <t>₹ 37,444</t>
+  </si>
+  <si>
+    <t>₹ 76,013</t>
+  </si>
+  <si>
+    <t>₹ 36,934</t>
   </si>
 </sst>
 </file>

</xml_diff>